<commit_message>
feat: Add Expenses, Sales Report
</commit_message>
<xml_diff>
--- a/public/template/report/Template_Report_Expenses_Summary.xlsx
+++ b/public/template/report/Template_Report_Expenses_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerjaan\Project\rpc-be\public\template\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D631C841-5C51-4AC9-A8B0-FC37B547E627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA96D942-7DEB-42B2-803F-EE47FF21D6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
   </bookViews>
@@ -25,52 +25,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Category</t>
   </si>
   <si>
-    <t>May 21</t>
-  </si>
-  <si>
-    <t>Jun 21</t>
-  </si>
-  <si>
-    <t>Jul 21</t>
-  </si>
-  <si>
-    <t>Aug 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sep 21 </t>
-  </si>
-  <si>
-    <t>Oct 21</t>
-  </si>
-  <si>
-    <t>Nov 21</t>
-  </si>
-  <si>
-    <t>Dec 21</t>
-  </si>
-  <si>
-    <t>Jan 22</t>
-  </si>
-  <si>
-    <t>Feb 22</t>
-  </si>
-  <si>
-    <t>Mar 22</t>
-  </si>
-  <si>
-    <t>Apr 22</t>
+    <t>Jan 24</t>
+  </si>
+  <si>
+    <t>Feb 24</t>
+  </si>
+  <si>
+    <t>Mar 24</t>
+  </si>
+  <si>
+    <t>Apr 24</t>
+  </si>
+  <si>
+    <t>Mei 24</t>
+  </si>
+  <si>
+    <t>Jun 24</t>
+  </si>
+  <si>
+    <t>Jul 24</t>
+  </si>
+  <si>
+    <t>Aug 24</t>
+  </si>
+  <si>
+    <t>Sep 24</t>
+  </si>
+  <si>
+    <t>Oct 24</t>
+  </si>
+  <si>
+    <t>Nov 24</t>
+  </si>
+  <si>
+    <t>Des 24</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,6 +93,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,11 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0BD312-7EF2-F445-B81C-635468D350A0}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B7" activeCellId="1" sqref="A5 B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -473,7 +485,7 @@
     <col min="9" max="9" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,8 +525,23 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="4">
+        <v>45658</v>
+      </c>
+      <c r="O1" s="4">
+        <v>45689</v>
+      </c>
+      <c r="P1" s="4">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>